<commit_message>
output multiple p_in and p_out based on different resistance
</commit_message>
<xml_diff>
--- a/wk.xlsx
+++ b/wk.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LYer\Git Repos\wk\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git Repos\wk\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -339,7 +339,7 @@
   <dimension ref="A1:B185"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B153"/>
+      <selection sqref="A1:B145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -354,1466 +354,1466 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>7.7087194244565853E-4</v>
+        <v>8.3948375889236402E-4</v>
       </c>
       <c r="B2">
-        <v>79.97971636612165</v>
+        <v>79.979887396867426</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>1.5417438848913171E-3</v>
+        <v>1.678967517784728E-3</v>
       </c>
       <c r="B3">
-        <v>80.060685358188266</v>
+        <v>80.061237374120765</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>2.3126158273369755E-3</v>
+        <v>2.5184512766770919E-3</v>
       </c>
       <c r="B4">
-        <v>80.142994931414393</v>
+        <v>80.14418192265812</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>3.0834877697826341E-3</v>
+        <v>3.3579350355694561E-3</v>
       </c>
       <c r="B5">
-        <v>80.226645085800044</v>
+        <v>80.228721042479478</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>3.8543597122282927E-3</v>
+        <v>4.1974187944618198E-3</v>
       </c>
       <c r="B6">
-        <v>80.31163582134522</v>
+        <v>80.314854733584838</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>4.6252316546739509E-3</v>
+        <v>5.0369025533541839E-3</v>
       </c>
       <c r="B7">
-        <v>80.397967138049907</v>
+        <v>80.402582995974214</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>5.39610359711961E-3</v>
+        <v>5.876386312246548E-3</v>
       </c>
       <c r="B8">
-        <v>80.485639035914119</v>
+        <v>80.491905829647607</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>6.1669755395652682E-3</v>
+        <v>6.7158700711389121E-3</v>
       </c>
       <c r="B9">
-        <v>80.574651514937855</v>
+        <v>80.582823234605002</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>7.7087194244565855E-3</v>
+        <v>8.3948375889236395E-3</v>
       </c>
       <c r="B10">
-        <v>80.756596255149873</v>
+        <v>80.769296867283146</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>9.2504633093479019E-3</v>
+        <v>1.0073805106708368E-2</v>
       </c>
       <c r="B11">
-        <v>80.943746783055417</v>
+        <v>80.961952290303302</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>1.079220719423922E-2</v>
+        <v>1.1752772624493094E-2</v>
       </c>
       <c r="B12">
-        <v>81.136011477270841</v>
+        <v>81.160658268012085</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>1.2333951079130535E-2</v>
+        <v>1.3431740142277823E-2</v>
       </c>
       <c r="B13">
-        <v>81.33332829821407</v>
+        <v>81.365332867797676</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>1.3875694964021853E-2</v>
+        <v>1.5110707660062551E-2</v>
       </c>
       <c r="B14">
-        <v>81.535635206303056</v>
+        <v>81.575894157048197</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>1.5417438848913171E-2</v>
+        <v>1.6789675177847279E-2</v>
       </c>
       <c r="B15">
-        <v>81.74287016195575</v>
+        <v>81.792260203151827</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>1.6959182733804486E-2</v>
+        <v>1.8468642695632007E-2</v>
       </c>
       <c r="B16">
-        <v>81.954971125590092</v>
+        <v>82.014349073496689</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>1.8500926618695804E-2</v>
+        <v>2.0147610213416735E-2</v>
       </c>
       <c r="B17">
-        <v>82.171876057624033</v>
+        <v>82.242078835470963</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>2.158441438847844E-2</v>
+        <v>2.3505545248986192E-2</v>
       </c>
       <c r="B18">
-        <v>82.619759419917997</v>
+        <v>82.713990902614441</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>2.4667902158261073E-2</v>
+        <v>2.6863480284555648E-2</v>
       </c>
       <c r="B19">
-        <v>83.086038536174783</v>
+        <v>83.207396820177394</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>2.7751389928043706E-2</v>
+        <v>3.0221415320125102E-2</v>
       </c>
       <c r="B20">
-        <v>83.570091558635696</v>
+        <v>83.721450037662109</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>3.0834877697826342E-2</v>
+        <v>3.3579350355694558E-2</v>
       </c>
       <c r="B21">
-        <v>84.071330129450033</v>
+        <v>84.255368081068454</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>3.3918365467608978E-2</v>
+        <v>3.6937285391264015E-2</v>
       </c>
       <c r="B22">
-        <v>84.589150112276627</v>
+        <v>84.808346702721082</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>3.7001853237391608E-2</v>
+        <v>4.0295220426833471E-2</v>
       </c>
       <c r="B23">
-        <v>85.122931592283919</v>
+        <v>85.379559881269401</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>4.0085341007174244E-2</v>
+        <v>4.3653155462402927E-2</v>
       </c>
       <c r="B24">
-        <v>85.672038876149855</v>
+        <v>85.968159821687678</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>4.316882877695688E-2</v>
+        <v>4.7011090497972384E-2</v>
       </c>
       <c r="B25">
-        <v>86.235820492061947</v>
+        <v>86.573276955274935</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>4.9335804316522153E-2</v>
+        <v>5.3726960569111297E-2</v>
       </c>
       <c r="B26">
-        <v>87.405092750779787</v>
+        <v>87.830180002423504</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>5.5502779856087418E-2</v>
+        <v>6.044283064025021E-2</v>
       </c>
       <c r="B27">
-        <v>88.624849931811056</v>
+        <v>89.142052076281317</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>6.1669755395652684E-2</v>
+        <v>6.7158700711389116E-2</v>
       </c>
       <c r="B28">
-        <v>89.889855012619861</v>
+        <v>90.502128051066364</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>6.7836730935217956E-2</v>
+        <v>7.3874570782528029E-2</v>
       </c>
       <c r="B29">
-        <v>91.194432381103226</v>
+        <v>91.902881034835858</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>7.4003706474783229E-2</v>
+        <v>8.0590440853666942E-2</v>
       </c>
       <c r="B30">
-        <v>92.532773078790171</v>
+        <v>93.336623412596069</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>8.0170682014348488E-2</v>
+        <v>8.7306310924805855E-2</v>
       </c>
       <c r="B31">
-        <v>93.898951229735317</v>
+        <v>94.795532729854372</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>8.633765755391376E-2</v>
+        <v>9.4022180995944768E-2</v>
       </c>
       <c r="B32">
-        <v>95.286940469412642</v>
+        <v>96.271677576171243</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>9.2504633093479033E-2</v>
+        <v>0.10073805106708368</v>
       </c>
       <c r="B33">
-        <v>96.690630373609068</v>
+        <v>97.75704346871234</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>0.1029212997601457</v>
+        <v>0.11115471773375035</v>
       </c>
       <c r="B34">
-        <v>99.081359889027823</v>
+        <v>100.06201698107417</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>0.11333796642681238</v>
+        <v>0.12157138440041702</v>
       </c>
       <c r="B35">
-        <v>101.46859026356347</v>
+        <v>102.33869806144929</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>0.12375463309347903</v>
+        <v>0.13198805106708369</v>
       </c>
       <c r="B36">
-        <v>103.82389022645056</v>
+        <v>104.55914489947521</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>0.13417129976014569</v>
+        <v>0.14240471773375035</v>
       </c>
       <c r="B37">
-        <v>106.11799188931668</v>
+        <v>106.69448332994827</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>0.14458796642681238</v>
+        <v>0.15282138440041704</v>
       </c>
       <c r="B38">
-        <v>108.3223124108367</v>
+        <v>108.71678317552532</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>0.15500463309347903</v>
+        <v>0.16323805106708369</v>
       </c>
       <c r="B39">
-        <v>110.40928482125514</v>
+        <v>110.59939059594113</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>0.16542129976014569</v>
+        <v>0.17365471773375035</v>
       </c>
       <c r="B40">
-        <v>112.35270012823152</v>
+        <v>112.31727062147705</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>0.17583796642681238</v>
+        <v>0.18407138440041704</v>
       </c>
       <c r="B41">
-        <v>114.12806070400882</v>
+        <v>113.84735987068102</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>0.18625463309347906</v>
+        <v>0.19448805106708372</v>
       </c>
       <c r="B42">
-        <v>115.70716540343665</v>
+        <v>115.16141314394255</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>0.19667129976014572</v>
+        <v>0.20490471773375038</v>
       </c>
       <c r="B43">
-        <v>117.07748790295165</v>
+        <v>116.25164124459543</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>0.20708796642681238</v>
+        <v>0.21532138440041704</v>
       </c>
       <c r="B44">
-        <v>118.21485331253696</v>
+        <v>117.09421000679217</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>0.21750463309347906</v>
+        <v>0.22573805106708372</v>
       </c>
       <c r="B45">
-        <v>119.10215508362467</v>
+        <v>117.67406745050671</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>0.22792129976014575</v>
+        <v>0.23615471773375041</v>
       </c>
       <c r="B46">
-        <v>119.72473441633703</v>
+        <v>117.97873933946551</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>0.2383379664268124</v>
+        <v>0.24657138440041707</v>
       </c>
       <c r="B47">
-        <v>120.07051412772816</v>
+        <v>117.99843793086113</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>0.24875463309347906</v>
+        <v>0.25698805106708372</v>
       </c>
       <c r="B48">
-        <v>120.13010303701061</v>
+        <v>117.72613879215622</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>0.25917129976014575</v>
+        <v>0.26740471773375041</v>
       </c>
       <c r="B49">
-        <v>119.89686823807672</v>
+        <v>117.15762304140488</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>0.26437963309347906</v>
+        <v>0.27261305106708372</v>
       </c>
       <c r="B50">
-        <v>119.66824612212692</v>
+        <v>116.76066121431266</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>0.26958796642681243</v>
+        <v>0.27782138440041709</v>
       </c>
       <c r="B51">
-        <v>119.36623004329353</v>
+        <v>116.29062679878</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>0.27479629976014575</v>
+        <v>0.28302971773375041</v>
       </c>
       <c r="B52">
-        <v>118.98987937862458</v>
+        <v>115.74668707725013</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>0.28000463309347912</v>
+        <v>0.28823805106708378</v>
       </c>
       <c r="B53">
-        <v>118.5393608734653</v>
+        <v>115.12932332873193</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>0.28521296642681243</v>
+        <v>0.29344638440041709</v>
       </c>
       <c r="B54">
-        <v>118.01501769751972</v>
+        <v>114.43919126660379</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55">
-        <v>0.29042129976014575</v>
+        <v>0.29865471773375041</v>
       </c>
       <c r="B55">
-        <v>117.41736716867044</v>
+        <v>113.67711777451083</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56">
-        <v>0.29562963309347912</v>
+        <v>0.30386305106708378</v>
       </c>
       <c r="B56">
-        <v>116.74709780927505</v>
+        <v>112.8440969519187</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57">
-        <v>0.30083796642681243</v>
+        <v>0.30907138440041709</v>
       </c>
       <c r="B57">
-        <v>116.00506571553825</v>
+        <v>111.94128545026985</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58">
-        <v>0.30604629976014575</v>
+        <v>0.31427971773375041</v>
       </c>
       <c r="B58">
-        <v>115.23108360474522</v>
+        <v>111.0170136795616</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59">
-        <v>0.31125463309347912</v>
+        <v>0.31948805106708378</v>
       </c>
       <c r="B59">
-        <v>114.40521031457826</v>
+        <v>110.04116669877399</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60">
-        <v>0.31646296642681243</v>
+        <v>0.32469638440041709</v>
       </c>
       <c r="B60">
-        <v>113.56895304206226</v>
+        <v>109.06381384112564</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61">
-        <v>0.32167129976014575</v>
+        <v>0.32990471773375041</v>
       </c>
       <c r="B61">
-        <v>112.74430772176595</v>
+        <v>108.10928013497511</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62">
-        <v>0.32687963309347912</v>
+        <v>0.33511305106708378</v>
       </c>
       <c r="B62">
-        <v>111.95739205772615</v>
+        <v>107.20637531656429</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63">
-        <v>0.33208796642681243</v>
+        <v>0.34032138440041709</v>
       </c>
       <c r="B63">
-        <v>111.23890251440174</v>
+        <v>106.38888929220067</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64">
-        <v>0.3372962997601458</v>
+        <v>0.34552971773375046</v>
       </c>
       <c r="B64">
-        <v>110.62460168825065</v>
+        <v>105.69612030539545</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65">
-        <v>0.34250463309347912</v>
+        <v>0.35073805106708378</v>
       </c>
       <c r="B65">
-        <v>110.15583697812411</v>
+        <v>105.17343678741264</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66">
-        <v>0.3451087997601458</v>
+        <v>0.35334221773375046</v>
       </c>
       <c r="B66">
-        <v>109.96404386648719</v>
+        <v>104.96014480724838</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67">
-        <v>0.34771296642681243</v>
+        <v>0.35594638440041709</v>
       </c>
       <c r="B67">
-        <v>109.79533852615246</v>
+        <v>104.77545635425354</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68">
-        <v>0.35031713309347912</v>
+        <v>0.35855055106708378</v>
       </c>
       <c r="B68">
-        <v>109.63760346947578</v>
+        <v>104.60374679364085</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69">
-        <v>0.35292129976014575</v>
+        <v>0.36115471773375041</v>
       </c>
       <c r="B69">
-        <v>109.48712159773918</v>
+        <v>104.44057191965899</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70">
-        <v>0.35552546642681243</v>
+        <v>0.36375888440041709</v>
       </c>
       <c r="B70">
-        <v>109.33932155271077</v>
+        <v>104.2805066685717</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71">
-        <v>0.35812963309347912</v>
+        <v>0.36636305106708378</v>
       </c>
       <c r="B71">
-        <v>109.18870492701596</v>
+        <v>104.11706254564936</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72">
-        <v>0.36073379976014575</v>
+        <v>0.36896721773375041</v>
       </c>
       <c r="B72">
-        <v>109.0287703573522</v>
+        <v>103.94260154104879</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73">
-        <v>0.36333796642681243</v>
+        <v>0.37157138440041709</v>
       </c>
       <c r="B73">
-        <v>108.8519344441153</v>
+        <v>103.74824647142557</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74">
-        <v>0.36594213309347912</v>
+        <v>0.37417555106708378</v>
       </c>
       <c r="B74">
-        <v>108.66793256368524</v>
+        <v>103.54663835813687</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75">
-        <v>0.36854629976014575</v>
+        <v>0.37677971773375041</v>
       </c>
       <c r="B75">
-        <v>108.47202370160394</v>
+        <v>103.32959427063609</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76">
-        <v>0.37115046642681243</v>
+        <v>0.37938388440041709</v>
       </c>
       <c r="B76">
-        <v>108.2712073969815</v>
+        <v>103.10662438356891</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77">
-        <v>0.37375463309347912</v>
+        <v>0.38198805106708378</v>
       </c>
       <c r="B77">
-        <v>108.06649776476105</v>
+        <v>102.87896996597944</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78">
-        <v>0.37635879976014575</v>
+        <v>0.38459221773375041</v>
       </c>
       <c r="B78">
-        <v>107.85971457922652</v>
+        <v>102.64884478796786</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79">
-        <v>0.37896296642681243</v>
+        <v>0.38719638440041709</v>
       </c>
       <c r="B79">
-        <v>107.65360808173415</v>
+        <v>102.41958361332178</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80">
-        <v>0.38156713309347906</v>
+        <v>0.38980055106708372</v>
       </c>
       <c r="B80">
-        <v>107.4519918701635</v>
+        <v>102.19580023955008</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81">
-        <v>0.38417129976014575</v>
+        <v>0.39240471773375041</v>
       </c>
       <c r="B81">
-        <v>107.25988407064845</v>
+        <v>101.98355532136422</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82">
-        <v>0.38677546642681243</v>
+        <v>0.39500888440041709</v>
       </c>
       <c r="B82">
-        <v>107.07168018747841</v>
+        <v>101.77525837248477</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83">
-        <v>0.38937963309347906</v>
+        <v>0.39761305106708372</v>
       </c>
       <c r="B83">
-        <v>106.89046146285234</v>
+        <v>101.5763485702998</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84">
-        <v>0.39198379976014575</v>
+        <v>0.40021721773375041</v>
       </c>
       <c r="B84">
-        <v>106.71210196680312</v>
+        <v>101.38099709894156</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85">
-        <v>0.39458796642681238</v>
+        <v>0.40282138440041704</v>
       </c>
       <c r="B85">
-        <v>106.53629831500588</v>
+        <v>101.18882380665661</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86">
-        <v>0.39719213309347906</v>
+        <v>0.40542555106708372</v>
       </c>
       <c r="B86">
-        <v>106.36229218663706</v>
+        <v>100.99888477976526</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87">
-        <v>0.39979629976014575</v>
+        <v>0.40802971773375041</v>
       </c>
       <c r="B87">
-        <v>106.1887561048068</v>
+        <v>100.80953157036896</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88">
-        <v>0.40240046642681238</v>
+        <v>0.41063388440041704</v>
       </c>
       <c r="B88">
-        <v>106.01366789832225</v>
+        <v>100.6182565794515</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89">
-        <v>0.40500463309347906</v>
+        <v>0.41323805106708372</v>
       </c>
       <c r="B89">
-        <v>105.83417343943289</v>
+        <v>100.42152410217673</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90">
-        <v>0.40760879976014575</v>
+        <v>0.41584221773375041</v>
       </c>
       <c r="B90">
-        <v>105.6529534682807</v>
+        <v>100.22306292726927</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91">
-        <v>0.41021296642681238</v>
+        <v>0.41844638440041704</v>
       </c>
       <c r="B91">
-        <v>105.46919761869141</v>
+        <v>100.02102304540183</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92">
-        <v>0.41281713309347906</v>
+        <v>0.42105055106708372</v>
       </c>
       <c r="B92">
-        <v>105.28477363694232</v>
+        <v>99.818133874400402</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93">
-        <v>0.41542129976014575</v>
+        <v>0.42365471773375041</v>
       </c>
       <c r="B93">
-        <v>105.09975769164191</v>
+        <v>99.614493201887171</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94">
-        <v>0.41802546642681238</v>
+        <v>0.42625888440041704</v>
       </c>
       <c r="B94">
-        <v>104.91441236668391</v>
+        <v>99.410435620885309</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95">
-        <v>0.42062963309347906</v>
+        <v>0.42886305106708372</v>
       </c>
       <c r="B95">
-        <v>104.72924552098972</v>
+        <v>99.206607082897378</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96">
-        <v>0.42323379976014569</v>
+        <v>0.43146721773375035</v>
       </c>
       <c r="B96">
-        <v>104.54507709525529</v>
+        <v>99.004049482773397</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97">
-        <v>0.42583796642681238</v>
+        <v>0.43407138440041704</v>
       </c>
       <c r="B97">
-        <v>104.36311426422644</v>
+        <v>98.804295775813898</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98">
-        <v>0.42844213309347906</v>
+        <v>0.43667555106708372</v>
       </c>
       <c r="B98">
-        <v>104.18291620209256</v>
+        <v>98.606778754340283</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99">
-        <v>0.43104629976014569</v>
+        <v>0.43927971773375035</v>
       </c>
       <c r="B99">
-        <v>104.00307127109131</v>
+        <v>98.409720030172906</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100">
-        <v>0.43365046642681238</v>
+        <v>0.44188388440041704</v>
       </c>
       <c r="B100">
-        <v>103.82355807233546</v>
+        <v>98.21308512552902</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101">
-        <v>0.43625463309347901</v>
+        <v>0.44448805106708367</v>
       </c>
       <c r="B101">
-        <v>103.64437253497704</v>
+        <v>98.016868236573629</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102">
-        <v>0.43885879976014569</v>
+        <v>0.44709221773375035</v>
       </c>
       <c r="B102">
-        <v>103.46550716586849</v>
+        <v>97.82105874665686</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103">
-        <v>0.44146296642681238</v>
+        <v>0.44969638440041704</v>
       </c>
       <c r="B103">
-        <v>103.2869503414983</v>
+        <v>97.625640233650827</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104">
-        <v>0.44406713309347901</v>
+        <v>0.45230055106708367</v>
       </c>
       <c r="B104">
-        <v>103.10868554920287</v>
+        <v>97.43058940633918</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105">
-        <v>0.44667129976014569</v>
+        <v>0.45490471773375035</v>
       </c>
       <c r="B105">
-        <v>102.93069057765457</v>
+        <v>97.235874969859339</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106">
-        <v>0.45187963309347901</v>
+        <v>0.46011305106708367</v>
       </c>
       <c r="B106">
-        <v>102.57558479023488</v>
+        <v>96.847567193354891</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107">
-        <v>0.45708796642681238</v>
+        <v>0.46532138440041704</v>
       </c>
       <c r="B107">
-        <v>102.22165612992492</v>
+        <v>96.460734852354335</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108">
-        <v>0.46229629976014569</v>
+        <v>0.47052971773375035</v>
       </c>
       <c r="B108">
-        <v>101.86892499355702</v>
+        <v>96.075413416933117</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109">
-        <v>0.46750463309347901</v>
+        <v>0.47573805106708367</v>
       </c>
       <c r="B109">
-        <v>101.51738860540652</v>
+        <v>95.691598820749761</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110">
-        <v>0.47271296642681238</v>
+        <v>0.48094638440041704</v>
       </c>
       <c r="B110">
-        <v>101.16704923749553</v>
+        <v>95.309294277746417</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111">
-        <v>0.47792129976014569</v>
+        <v>0.48615471773375035</v>
       </c>
       <c r="B111">
-        <v>100.81791527437144</v>
+        <v>94.928511813647361</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112">
-        <v>0.48312963309347906</v>
+        <v>0.49136305106708372</v>
       </c>
       <c r="B112">
-        <v>100.47000227788563</v>
+        <v>94.549273797457431</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113">
-        <v>0.48833796642681238</v>
+        <v>0.49657138440041704</v>
       </c>
       <c r="B113">
-        <v>100.12333405197199</v>
+        <v>94.171614472960513</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114">
-        <v>0.49875463309347906</v>
+        <v>0.50698805106708367</v>
       </c>
       <c r="B114">
-        <v>99.433650388066155</v>
+        <v>93.420914372559977</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115">
-        <v>0.50917129976014575</v>
+        <v>0.51740471773375041</v>
       </c>
       <c r="B115">
-        <v>98.74871849301401</v>
+        <v>92.676199917272641</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116">
-        <v>0.51958796642681238</v>
+        <v>0.52782138440041704</v>
       </c>
       <c r="B116">
-        <v>98.068505968731273</v>
+        <v>91.937424215983043</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117">
-        <v>0.53000463309347912</v>
+        <v>0.53823805106708367</v>
       </c>
       <c r="B117">
-        <v>97.392979969322994</v>
+        <v>91.204539373194933</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118">
-        <v>0.54042129976014575</v>
+        <v>0.54865471773375041</v>
       </c>
       <c r="B118">
-        <v>96.722107695134</v>
+        <v>90.477497581457925</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119">
-        <v>0.55083796642681238</v>
+        <v>0.55907138440041704</v>
       </c>
       <c r="B119">
-        <v>96.055856392748836</v>
+        <v>89.756251121367555</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120">
-        <v>0.56125463309347912</v>
+        <v>0.56948805106708378</v>
       </c>
       <c r="B120">
-        <v>95.394193354991828</v>
+        <v>89.040752361565211</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121">
-        <v>0.57167129976014575</v>
+        <v>0.57990471773375041</v>
       </c>
       <c r="B121">
-        <v>94.737085920926987</v>
+        <v>88.330953758738218</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122">
-        <v>0.58208796642681238</v>
+        <v>0.59032138440041704</v>
       </c>
       <c r="B122">
-        <v>94.084509504821014</v>
+        <v>87.626822954267993</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123">
-        <v>0.59250463309347912</v>
+        <v>0.60073805106708378</v>
       </c>
       <c r="B123">
-        <v>93.436421794881284</v>
+        <v>86.928292665612631</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124">
-        <v>0.60292129976014575</v>
+        <v>0.61115471773375041</v>
       </c>
       <c r="B124">
-        <v>92.792798105682579</v>
+        <v>86.235330397456565</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125">
-        <v>0.61333796642681238</v>
+        <v>0.62157138440041715</v>
       </c>
       <c r="B125">
-        <v>92.153607747629891</v>
+        <v>85.547891866284772</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126">
-        <v>0.62375463309347912</v>
+        <v>0.63198805106708378</v>
       </c>
       <c r="B126">
-        <v>91.518820272245989</v>
+        <v>84.865933193822485</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127">
-        <v>0.63417129976014575</v>
+        <v>0.64240471773375041</v>
       </c>
       <c r="B127">
-        <v>90.888405472171428</v>
+        <v>84.189410907034997</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128">
-        <v>0.64458796642681249</v>
+        <v>0.65282138440041715</v>
       </c>
       <c r="B128">
-        <v>90.262333381164552</v>
+        <v>83.518281938127814</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129">
-        <v>0.65500463309347912</v>
+        <v>0.66323805106708378</v>
       </c>
       <c r="B129">
-        <v>89.640574274101454</v>
+        <v>82.852503624546614</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130">
-        <v>0.66542129976014575</v>
+        <v>0.67365471773375041</v>
       </c>
       <c r="B130">
-        <v>89.023105124783569</v>
+        <v>82.192046292950494</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131">
-        <v>0.67583796642681249</v>
+        <v>0.68407138440041715</v>
       </c>
       <c r="B131">
-        <v>88.409882471027132</v>
+        <v>81.536840625249155</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132">
-        <v>0.68625463309347912</v>
+        <v>0.69448805106708378</v>
       </c>
       <c r="B132">
-        <v>87.800883847840836</v>
+        <v>80.886857897789852</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133">
-        <v>0.69667129976014586</v>
+        <v>0.70490471773375041</v>
       </c>
       <c r="B133">
-        <v>87.196080168328137</v>
+        <v>80.242056493890928</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134">
-        <v>0.70708796642681249</v>
+        <v>0.71532138440041715</v>
       </c>
       <c r="B134">
-        <v>86.59544255563948</v>
+        <v>79.602395147340602</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135">
-        <v>0.71750463309347912</v>
+        <v>0.72573805106708378</v>
       </c>
       <c r="B135">
-        <v>85.998942342972242</v>
+        <v>78.96783294239701</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136">
-        <v>0.72792129976014586</v>
+        <v>0.73615471773375052</v>
       </c>
       <c r="B136">
-        <v>85.406551073570697</v>
+        <v>78.338329313788151</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137">
-        <v>0.73833796642681249</v>
+        <v>0.74657138440041715</v>
       </c>
       <c r="B137">
-        <v>84.818240500726148</v>
+        <v>77.713844046711898</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138">
-        <v>0.74875463309347912</v>
+        <v>0.75741662801703169</v>
       </c>
       <c r="B138">
-        <v>84.233988935673082</v>
+        <v>77.068968792749558</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139">
-        <v>0.75917129976014586</v>
+        <v>0.76826187163364623</v>
       </c>
       <c r="B139">
-        <v>83.653755400286855</v>
+        <v>76.429430502411648</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140">
-        <v>0.76958796642681249</v>
+        <v>0.77910711525026077</v>
       </c>
       <c r="B140">
-        <v>83.077518653501372</v>
+        <v>75.795199120319936</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141">
-        <v>0.78000463309347912</v>
+        <v>0.78995235886687531</v>
       </c>
       <c r="B141">
-        <v>82.505251174753255</v>
+        <v>75.166230630679564</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142">
-        <v>0.79042129976014586</v>
+        <v>0.80079760248348975</v>
       </c>
       <c r="B142">
-        <v>81.936925642664846</v>
+        <v>74.54248140465252</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143">
-        <v>0.80083796642681249</v>
+        <v>0.81164284610010429</v>
       </c>
       <c r="B143">
-        <v>81.372514935044293</v>
+        <v>73.923908200357587</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144">
-        <v>0.81125463309347923</v>
+        <v>0.82248808971671883</v>
       </c>
       <c r="B144">
-        <v>80.811992128885478</v>
+        <v>73.310468162870379</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145">
-        <v>0.82167129976014586</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="B145">
-        <v>80.255330500368046</v>
+        <v>72.702118824223319</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146">
-        <v>0.82312905395679425</v>
+        <v>0.52401459799926253</v>
       </c>
       <c r="B146">
-        <v>80.177735291976816</v>
+        <v>93.153902093084369</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147">
-        <v>0.82458680815344276</v>
+        <v>0.53443126466592927</v>
       </c>
       <c r="B147">
-        <v>80.100215107287312</v>
+        <v>92.411316483873421</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148">
-        <v>0.82604456235009116</v>
+        <v>0.5448479313325959</v>
       </c>
       <c r="B148">
-        <v>80.022769873312001</v>
+        <v>91.674654029331279</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149">
-        <v>0.82750231654673967</v>
+        <v>0.55526459799926253</v>
       </c>
       <c r="B149">
-        <v>79.945399517587731</v>
+        <v>90.943866575781541</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150">
-        <v>0.82896007074338807</v>
+        <v>0.56568126466592927</v>
       </c>
       <c r="B150">
-        <v>79.868103967721368</v>
+        <v>90.218905969547805</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151">
-        <v>0.83041782494003646</v>
+        <v>0.5760979313325959</v>
       </c>
       <c r="B151">
-        <v>79.790883151389764</v>
+        <v>89.499724056953681</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152">
-        <v>0.83187557913668497</v>
+        <v>0.58651459799926264</v>
       </c>
       <c r="B152">
-        <v>79.713736996339648</v>
+        <v>88.786272684322768</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153">
-        <v>0.83333333333333337</v>
+        <v>0.59693126466592927</v>
       </c>
       <c r="B153">
-        <v>79.63666543038758</v>
+        <v>88.07850369797869</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154">
-        <v>0.53203802210246465</v>
+        <v>0.6073479313325959</v>
       </c>
       <c r="B154">
-        <v>108.45483294886631</v>
+        <v>87.37611123440513</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155">
-        <v>0.54245468876913139</v>
+        <v>0.61776459799926264</v>
       </c>
       <c r="B155">
-        <v>107.31972970719559</v>
+        <v>86.679583901846485</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156">
-        <v>0.55287135543579802</v>
+        <v>0.62818126466592927</v>
       </c>
       <c r="B156">
-        <v>106.1965247224216</v>
+        <v>85.98861236246816</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157">
-        <v>0.56328802210246476</v>
+        <v>0.63859793133259601</v>
       </c>
       <c r="B157">
-        <v>105.08509016955328</v>
+        <v>85.303151440580848</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158">
-        <v>0.57370468876913139</v>
+        <v>0.64901459799926264</v>
       </c>
       <c r="B158">
-        <v>103.98529822359959</v>
+        <v>84.623155960495311</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159">
-        <v>0.58412135543579802</v>
+        <v>0.65943126466592927</v>
       </c>
       <c r="B159">
-        <v>102.89702105956943</v>
+        <v>83.948580746522225</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160">
-        <v>0.59453802210246476</v>
+        <v>0.66984793133259601</v>
       </c>
       <c r="B160">
-        <v>101.82013085247172</v>
+        <v>83.279380622972326</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161">
-        <v>0.60495468876913139</v>
+        <v>0.68026459799926264</v>
       </c>
       <c r="B161">
-        <v>100.75449977731546</v>
+        <v>82.615510414156333</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162">
-        <v>0.61537135543579802</v>
+        <v>0.69068126466592927</v>
       </c>
       <c r="B162">
-        <v>99.699110430727984</v>
+        <v>81.956942244336702</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163">
-        <v>0.62578802210246476</v>
+        <v>0.70109793133259601</v>
       </c>
       <c r="B163">
-        <v>98.655687821193169</v>
+        <v>81.303610905136637</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164">
-        <v>0.63620468876913139</v>
+        <v>0.71151459799926264</v>
       </c>
       <c r="B164">
-        <v>97.623202551455108</v>
+        <v>80.655487638395371</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165">
-        <v>0.64662135543579802</v>
+        <v>0.72193126466592927</v>
       </c>
       <c r="B165">
-        <v>96.601537076994134</v>
+        <v>80.012530913844131</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166">
-        <v>0.65703802210246476</v>
+        <v>0.73234793133259601</v>
       </c>
       <c r="B166">
-        <v>95.590573853290607</v>
+        <v>79.37469954839699</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167">
-        <v>0.66745468876913139</v>
+        <v>0.74276459799926264</v>
       </c>
       <c r="B167">
-        <v>94.590195335824873</v>
+        <v>78.741952706150983</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A168">
-        <v>0.67787135543579813</v>
+        <v>0.75318126466592938</v>
       </c>
       <c r="B168">
-        <v>93.600283980077279</v>
+        <v>78.114249898385978</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169">
-        <v>0.68828802210246476</v>
+        <v>0.76359793133259601</v>
       </c>
       <c r="B169">
-        <v>92.620722241528213</v>
+        <v>77.491550983564807</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170">
-        <v>0.69870468876913139</v>
+        <v>0.77231485658268817</v>
       </c>
       <c r="B170">
-        <v>91.65146544756756</v>
+        <v>76.974284538271718</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171">
-        <v>0.70912135543579813</v>
+        <v>0.78103178183278033</v>
       </c>
       <c r="B171">
-        <v>90.692299523965431</v>
+        <v>76.460464143698161</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172">
-        <v>0.71953802210246476</v>
+        <v>0.78974870708287248</v>
       </c>
       <c r="B172">
-        <v>89.743176816919473</v>
+        <v>75.950073528999809</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173">
-        <v>0.7299546887691315</v>
+        <v>0.79846563233296464</v>
       </c>
       <c r="B173">
-        <v>88.803992097655225</v>
+        <v>75.443089818526559</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A174">
-        <v>0.74037135543579813</v>
+        <v>0.8071825575830569</v>
       </c>
       <c r="B174">
-        <v>87.87464131032641</v>
+        <v>74.939490299983618</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175">
-        <v>0.75078802210246476</v>
+        <v>0.81589948283314906</v>
       </c>
       <c r="B175">
-        <v>86.955021572014829</v>
+        <v>74.439252424431587</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A176">
-        <v>0.7612046887691315</v>
+        <v>0.82461640808324121</v>
       </c>
       <c r="B176">
-        <v>86.04503117273039</v>
+        <v>73.942353806286306</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A177">
-        <v>0.77162135543579813</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="B177">
-        <v>85.14456957541114</v>
+        <v>73.448772223319011</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A178">
-        <v>0.77933535267299003</v>
+        <v>0.78148730332412453</v>
       </c>
       <c r="B178">
-        <v>84.48384026219901</v>
+        <v>75.718578018090724</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A179">
-        <v>0.78704934991018194</v>
+        <v>0.78889387903972585</v>
       </c>
       <c r="B179">
-        <v>83.828221536292276</v>
+        <v>75.288902500904967</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A180">
-        <v>0.79476334714737384</v>
+        <v>0.79630045475532707</v>
       </c>
       <c r="B180">
-        <v>83.177693324152969</v>
+        <v>74.861665226076056</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A181">
-        <v>0.80247734438456575</v>
+        <v>0.8037070304709284</v>
       </c>
       <c r="B181">
-        <v>82.532216161078395</v>
+        <v>74.436852360436831</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A182">
-        <v>0.81019134162175765</v>
+        <v>0.81111360618652961</v>
       </c>
       <c r="B182">
-        <v>81.891750917741149</v>
+        <v>74.014450150558218</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A183">
-        <v>0.81790533885894956</v>
+        <v>0.81852018190213083</v>
       </c>
       <c r="B183">
-        <v>81.256258800189059</v>
+        <v>73.594444922394217</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A184">
-        <v>0.82561933609614147</v>
+        <v>0.82592675761773215</v>
       </c>
       <c r="B184">
-        <v>80.625701349845215</v>
+        <v>73.176823080926837</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.25">
@@ -1821,7 +1821,7 @@
         <v>0.83333333333333337</v>
       </c>
       <c r="B185">
-        <v>80.000040443507942</v>
+        <v>72.761571109811129</v>
       </c>
     </row>
   </sheetData>

</xml_diff>